<commit_message>
Xml Improvement and Case searching
</commit_message>
<xml_diff>
--- a/Info_Data.xlsx
+++ b/Info_Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C05662-07FC-4538-8271-EADC41576F1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9118BF47-F87C-4B39-A204-6657127C8787}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Variable</t>
   </si>
@@ -40,15 +40,9 @@
     <t>CaseNumber</t>
   </si>
   <si>
-    <t>7755000006</t>
-  </si>
-  <si>
     <t>CaseNumber2</t>
   </si>
   <si>
-    <t>7755000007</t>
-  </si>
-  <si>
     <t>Amitthakur</t>
   </si>
   <si>
@@ -56,6 +50,18 @@
   </si>
   <si>
     <t>Aamit5555500000@@</t>
+  </si>
+  <si>
+    <t>https://smartnsc.com/</t>
+  </si>
+  <si>
+    <t>Aamit55555000@</t>
+  </si>
+  <si>
+    <t>7744000279</t>
+  </si>
+  <si>
+    <t>7755000008</t>
   </si>
 </sst>
 </file>
@@ -402,19 +408,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -422,48 +430,72 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{E936C6EB-F756-4A8B-8FE4-44F24C392264}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{39685802-C8A3-4001-8966-40815C779CB6}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{E79D8086-5A85-405D-9532-1BA86352F883}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{07D802F0-E813-4010-B6E9-2E1849BFBDC7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Usda Case Wizard Completion
</commit_message>
<xml_diff>
--- a/Info_Data.xlsx
+++ b/Info_Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598FD66A-7C04-477E-8E99-EC8E4BF708F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A18123F-F616-4943-BCE4-1B2F2B675F24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -461,7 +461,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -478,15 +478,15 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>